<commit_message>
Sales BI Report by Imam Hossain With Source\3. Delivery Status
</commit_message>
<xml_diff>
--- a/2. Sales BI Report by Imam Hossain With Source/Code, Code Flow, Function with Notes, Learning Source (Sales BI by IM from Source).xlsx
+++ b/2. Sales BI Report by Imam Hossain With Source/Code, Code Flow, Function with Notes, Learning Source (Sales BI by IM from Source).xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Imam Hossain\IDoc\Power BI by IM\2. Sales BI Report by Imam Hossain With Source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F117091B-AE46-4E64-8FE3-10DC6C0C7104}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C455F628-9753-4810-A521-6A51ADDFBC4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="796" activeTab="2" xr2:uid="{BA506BA8-62E4-42EB-93AD-9835F75A9973}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="796" activeTab="3" xr2:uid="{BA506BA8-62E4-42EB-93AD-9835F75A9973}"/>
   </bookViews>
   <sheets>
     <sheet name="Calendar Date" sheetId="1" r:id="rId1"/>
     <sheet name="Last Refresh Date &amp; Time" sheetId="2" r:id="rId2"/>
     <sheet name="2. Sales Status" sheetId="8" r:id="rId3"/>
+    <sheet name="3. Delivery Status" sheetId="9" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="118">
   <si>
     <t>https://debug.to/899/calendarauto-function-can-not-find-a-base-column-of-datetime-type-in-the-model</t>
   </si>
@@ -2401,6 +2402,2366 @@
         <family val="3"/>
       </rPr>
       <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Weekday = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF3165BB"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>SWITCH</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF3165BB"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TRUE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(),</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"W 1"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>" W 2"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"  W 3"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"   W 4"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"    W 5"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"     W 6"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"      W 7"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"       W 8"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"        W 9"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"        W 10"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"         W 11"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>12</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"          W 12"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>13</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"           W 13"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>14</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"            W 14"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>15</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"             W 15"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>16</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"              W 16"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>17</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"               W 17"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>18</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"                W 18"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>19</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"                 W 19"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"                  W 20"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>21</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"                   W 21"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>22</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"                    W 22"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>23</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"                     W 23"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>24</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"                      W 24"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>25</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"                       W 25"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>26</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"                        W 26"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>27</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"                         W 27"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>28</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"                          W 28"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>29</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"                           W 29"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>30</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"                            W 30"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>31</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"                             W 31"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>32</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"                              W 32"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>33</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"                               W 33"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>34</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"                                W 34"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>35</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"                                 W 35"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>36</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"                                  W 36"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>37</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"                                   W 37"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>38</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"                                    W 38"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>39</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"                                     W 39"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>40</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"                                      W 40"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>41</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"                                       W 41"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>42</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"                                        W 42"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>43</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"                                         W 43"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>44</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"                                          W 44"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>45</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"                                           W 45"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>46</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"                                            W 46"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>47</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"                                             W 47"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>48</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"                                              W 48"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>49</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"                                               W 49"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>50</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"                                                W 50"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>51</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"                                                 W 51"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>52</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"                                                  W 52"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>53</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"                                                   W 53"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>54</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"                                                    W 54"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>55</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"                                                     W 55"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vw_OrderReconInfo[Week]=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>56</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"                                                      W 56"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">COST SHIPMENT = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF001080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Vw_OrderReconInfo[QTYShip]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF001080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Vw_OrderReconInfo[UNITPRICE]</t>
     </r>
   </si>
 </sst>
@@ -2494,7 +4855,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2504,6 +4865,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2638,7 +5005,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2687,16 +5054,25 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2817,16 +5193,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>39</xdr:col>
-      <xdr:colOff>493068</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>170558</xdr:rowOff>
+      <xdr:col>45</xdr:col>
+      <xdr:colOff>359718</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>75308</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2849,8 +5225,58 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6410325" y="1600200"/>
+          <a:off x="9934575" y="3429000"/>
           <a:ext cx="17857143" cy="7133333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2FD8AC47-5BA1-2AF0-CDF0-3F2110DFD21A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7858125" y="4400550"/>
+          <a:ext cx="5381625" cy="9515475"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3360,8 +5786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2172347E-957E-473A-A572-DC1F11BB6C8F}">
   <dimension ref="A2:M46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3414,7 +5840,7 @@
     </row>
     <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="27" t="s">
         <v>32</v>
       </c>
       <c r="C9" s="13"/>
@@ -3460,64 +5886,24 @@
       <c r="B13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="27"/>
-      <c r="K13" s="27"/>
-      <c r="L13" s="27"/>
       <c r="M13" s="4"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B14" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
-      <c r="I14" s="27"/>
-      <c r="J14" s="27"/>
-      <c r="K14" s="27"/>
-      <c r="L14" s="27"/>
       <c r="M14" s="4"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B15" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="27"/>
-      <c r="I15" s="27"/>
-      <c r="J15" s="27"/>
-      <c r="K15" s="27"/>
-      <c r="L15" s="27"/>
       <c r="M15" s="4"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B16" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="27"/>
-      <c r="K16" s="27"/>
-      <c r="L16" s="27"/>
       <c r="M16" s="4"/>
     </row>
     <row r="17" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3560,62 +5946,62 @@
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B26" s="29" t="s">
+      <c r="B26" s="28" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B27" s="29" t="s">
+      <c r="B27" s="28" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B28" s="29" t="s">
+      <c r="B28" s="28" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B29" s="29" t="s">
+      <c r="B29" s="28" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B30" s="29" t="s">
+      <c r="B30" s="28" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B31" s="29" t="s">
+      <c r="B31" s="28" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B32" s="29" t="s">
+      <c r="B32" s="28" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="29" t="s">
+      <c r="B33" s="28" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="29" t="s">
+      <c r="B34" s="28" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" s="29" t="s">
+      <c r="B35" s="28" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B36" s="29" t="s">
+      <c r="B36" s="28" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B37" s="29" t="s">
+      <c r="B37" s="28" t="s">
         <v>54</v>
       </c>
     </row>
@@ -3654,4 +6040,406 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AD7A95B-549E-440D-9AB9-543F7BC4566F}">
+  <dimension ref="A2:A83"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="J79" sqref="J79"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="22" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="22" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="22" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="22" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="22" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="22" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="22" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="22" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="22" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="22" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="22" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="22" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="22" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="22" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="22" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="22" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="22" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="22" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="22" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="22" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="22" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="22" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="22" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="22" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="22" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="22" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="22" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="22" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="22" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="22" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="22" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="22" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="22" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="22" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="22" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="22" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="22" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="22" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="22" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="22" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="22" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="22" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="22" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="22" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="22" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="22" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="22" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="22" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="29"/>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="62" spans="1:1" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="64" spans="1:1" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="20" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="66" spans="1:1" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="30" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="70" spans="1:1" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="31" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="31" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="31" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="31" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="31" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="31" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="31" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="31" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="31" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="31" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="31" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="31" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Sales BI Report by Imam Hossain With Source\4. Shipment Details
</commit_message>
<xml_diff>
--- a/2. Sales BI Report by Imam Hossain With Source/Code, Code Flow, Function with Notes, Learning Source (Sales BI by IM from Source).xlsx
+++ b/2. Sales BI Report by Imam Hossain With Source/Code, Code Flow, Function with Notes, Learning Source (Sales BI by IM from Source).xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Imam Hossain\IDoc\Power BI by IM\2. Sales BI Report by Imam Hossain With Source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C455F628-9753-4810-A521-6A51ADDFBC4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A97456B2-9AFE-46F1-8047-372FBD9BA05C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="796" activeTab="3" xr2:uid="{BA506BA8-62E4-42EB-93AD-9835F75A9973}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="796" activeTab="4" xr2:uid="{BA506BA8-62E4-42EB-93AD-9835F75A9973}"/>
   </bookViews>
   <sheets>
     <sheet name="Calendar Date" sheetId="1" r:id="rId1"/>
     <sheet name="Last Refresh Date &amp; Time" sheetId="2" r:id="rId2"/>
     <sheet name="2. Sales Status" sheetId="8" r:id="rId3"/>
     <sheet name="3. Delivery Status" sheetId="9" r:id="rId4"/>
+    <sheet name="4. Shipment Details" sheetId="10" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="127">
   <si>
     <t>https://debug.to/899/calendarauto-function-can-not-find-a-base-column-of-datetime-type-in-the-model</t>
   </si>
@@ -4762,6 +4763,1068 @@
         <family val="3"/>
       </rPr>
       <t>Vw_OrderReconInfo[UNITPRICE]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ship Elie 1 = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF3165BB"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>SUMX</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF3165BB"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>FILTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF001080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'vw_Delivery Statement'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF001080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'vw_Delivery Statement'[LOCATION]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"FABEL1"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">), </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF001080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'vw_Delivery Statement'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF68349C"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[Ship Qty]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ship Elite = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF3165BB"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>( (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF3165BB"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>SUM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">('vw_Delivery Statement'[QTYSHIPPED]) - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF3165BB"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>SUMX</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF3165BB"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>FILTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">('vw_Delivery Statement', 'vw_Delivery Statement'[LOCATION] = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"FABSAM"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>), 'vw_Delivery Statement'[Ship Qty])) &lt;=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF3165BB"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>SUM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">('vw_Delivery Statement'[QTYSHIPPED]) - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF3165BB"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>SUMX</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF3165BB"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>FILTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">('vw_Delivery Statement', 'vw_Delivery Statement'[LOCATION] = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"FABSAM"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">), 'vw_Delivery Statement'[Ship Qty]))) </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ship Elite Cost = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF3165BB"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>( (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF3165BB"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>SUM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">('vw_Delivery Statement'[Total Cost]) - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF3165BB"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>SUMX</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF3165BB"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>FILTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">('vw_Delivery Statement', 'vw_Delivery Statement'[LOCATION] = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"FABSAM"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>), 'vw_Delivery Statement'[Ship Qty Cost])) &lt;=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF3165BB"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>SUM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">('vw_Delivery Statement'[Total Cost]) - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF3165BB"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>SUMX</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF3165BB"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>FILTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">('vw_Delivery Statement', 'vw_Delivery Statement'[LOCATION] = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"FABSAM"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>), 'vw_Delivery Statement'[Ship Qty Cost])))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ship Elite Qty = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF001080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'vw_Delivery Statement'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF68349C"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[Ship Elite]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ship Qty = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF3165BB"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>SUM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF001080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'vw_Delivery Statement'[QTYSHIPPED]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ship Qty Cost = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF3165BB"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>SUM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF001080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'vw_Delivery Statement'[Total Cost]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ship Sampl = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF3165BB"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> ( (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF3165BB"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>SUMX</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF3165BB"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>FILTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF001080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'vw_Delivery Statement'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF001080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'vw_Delivery Statement'[LOCATION]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"FABSAM"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">), </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF001080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'vw_Delivery Statement'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF68349C"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[Ship Qty]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)) =</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF3165BB"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>BLANK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(),</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF3165BB"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>SUMX</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF3165BB"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>FILTER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF001080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'vw_Delivery Statement'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF001080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'vw_Delivery Statement'[LOCATION]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"FABSAM"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">), </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF001080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'vw_Delivery Statement'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF68349C"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[Ship Qty]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">)) ) </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Shipment Value = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF3165BB"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>SUM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF001080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'vw_Delivery Statement'[Total Cost]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Total Export FAB = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF3165BB"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>CALCULATE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF3165BB"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>SUM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF001080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'vw_Delivery Statement'[QTYSHIPPED]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>),</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF001080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'vw_Delivery Statement'[LOCATION]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"FABEXP"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
     </r>
   </si>
 </sst>
@@ -4769,7 +5832,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4851,6 +5914,12 @@
     <font>
       <sz val="14"/>
       <color rgb="FF001080"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF68349C"/>
       <name val="Consolas"/>
       <family val="3"/>
     </font>
@@ -5005,7 +6074,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -5072,7 +6141,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -6046,7 +7114,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AD7A95B-549E-440D-9AB9-543F7BC4566F}">
   <dimension ref="A2:A83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+    <sheetView topLeftCell="A52" workbookViewId="0">
       <selection activeCell="J79" sqref="J79"/>
     </sheetView>
   </sheetViews>
@@ -6374,62 +7442,62 @@
         <v>42</v>
       </c>
     </row>
-    <row r="71" spans="1:1" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="31" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="72" spans="1:1" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="31" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="73" spans="1:1" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="31" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="74" spans="1:1" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="31" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="75" spans="1:1" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="31" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="76" spans="1:1" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="31" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="77" spans="1:1" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="31" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="78" spans="1:1" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="31" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="79" spans="1:1" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="31" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="80" spans="1:1" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="31" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="81" spans="1:1" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="31" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="82" spans="1:1" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="31" t="s">
         <v>54</v>
       </c>
@@ -6437,6 +7505,66 @@
     <row r="83" spans="1:1" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="19" t="s">
         <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55E0E4DE-43B6-414E-87C6-B5715EE19175}">
+  <dimension ref="A1:A17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="22" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="22" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="22" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="22" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="22" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>